<commit_message>
Update 216, 216 y 767
</commit_message>
<xml_diff>
--- a/Importación RETPER SOS.xlsx
+++ b/Importación RETPER SOS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF75533-235F-4191-84F4-9A37442AE4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E14154-E4D9-46CB-9A81-3C0BA2DC4BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Clientes!$A$1:$R$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Clientes!$A$1:$S$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="155">
   <si>
     <t>Nro</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Periodo</t>
   </si>
   <si>
-    <t>Desde (No Formula)</t>
-  </si>
-  <si>
     <t>Importar</t>
   </si>
   <si>
@@ -491,6 +488,12 @@
   </si>
   <si>
     <t>Destino</t>
+  </si>
+  <si>
+    <t>Raiz Destino</t>
+  </si>
+  <si>
+    <t>Desde</t>
   </si>
 </sst>
 </file>
@@ -904,11 +907,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R75"/>
+  <dimension ref="A1:S75"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,10 +920,10 @@
     <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="12" max="17" width="18" customWidth="1"/>
+    <col min="13" max="18" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -934,55 +937,58 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>153</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
         <f t="shared" ref="A2:A65" si="0">RIGHT(D2,1)</f>
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>20168291680</v>
@@ -995,45 +1001,46 @@
         <v>44958</v>
       </c>
       <c r="G2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H2" s="4" t="str">
         <f>G2&amp;"\"&amp;B2&amp;"\"&amp;YEAR(E2)&amp;"\"&amp;TEXT(MONTH(E2),"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\CRIVELLO LUIS\2023\02\</v>
       </c>
       <c r="I2" s="4"/>
-      <c r="J2" s="4" t="str">
+      <c r="J2" s="4"/>
+      <c r="K2" s="4" t="str">
         <f>TEXT(E2,"AAAAMM")</f>
         <v>202302</v>
       </c>
-      <c r="K2" s="3" t="str">
+      <c r="L2" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E2,"MMMM AAAA"),1))&amp;MID(TEXT(E2,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3" t="str">
-        <f>CONCATENATE(TEXT(A2,"0")," - ",SUBSTITUTE(D2,"-","")," - ",TEXT(K2,"AAAAMM")," - ",B2)</f>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3" t="str">
+        <f>CONCATENATE(TEXT(A2,"0")," - ",SUBSTITUTE(D2,"-","")," - ",TEXT(L2,"AAAAMM")," - ",B2)</f>
         <v>0 - 20168291680 - 202302 - CRIVELLO LUIS</v>
       </c>
-      <c r="N2" s="3" t="str">
-        <f>CONCATENATE(TEXT(A2,"0")," - ",SUBSTITUTE(D2,"-","")," - ",TEXT(K2,"AAAAMM")," - ",B2)</f>
+      <c r="O2" s="3" t="str">
+        <f>CONCATENATE(TEXT(A2,"0")," - ",SUBSTITUTE(D2,"-","")," - ",TEXT(L2,"AAAAMM")," - ",B2)</f>
         <v>0 - 20168291680 - 202302 - CRIVELLO LUIS</v>
       </c>
-      <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
-      <c r="R2" s="4">
+      <c r="R2" s="3"/>
+      <c r="S2" s="4">
         <f>ROW(A2)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>20315731330</v>
@@ -1046,348 +1053,355 @@
         <v>44958</v>
       </c>
       <c r="G3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H3" s="4" t="str">
         <f t="shared" ref="H3:H66" si="1">G3&amp;"\"&amp;B3&amp;"\"&amp;YEAR(E3)&amp;"\"&amp;TEXT(MONTH(E3),"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\VARENIZA ANGEL\2023\02\</v>
       </c>
       <c r="I3" s="4"/>
-      <c r="J3" s="4" t="str">
-        <f t="shared" ref="J3:J66" si="2">TEXT(E3,"AAAAMM")</f>
-        <v>202302</v>
-      </c>
-      <c r="K3" s="3" t="str">
+      <c r="J3" s="4"/>
+      <c r="K3" s="4" t="str">
+        <f t="shared" ref="K3:K66" si="2">TEXT(E3,"AAAAMM")</f>
+        <v>202302</v>
+      </c>
+      <c r="L3" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E3,"MMMM AAAA"),1))&amp;MID(TEXT(E3,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3" t="str">
-        <f t="shared" ref="M3:M66" si="3">CONCATENATE(TEXT(A3,"0")," - ",SUBSTITUTE(D3,"-","")," - ",TEXT(K3,"AAAAMM")," - ",B3)</f>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3" t="str">
+        <f t="shared" ref="N3:N66" si="3">CONCATENATE(TEXT(A3,"0")," - ",SUBSTITUTE(D3,"-","")," - ",TEXT(L3,"AAAAMM")," - ",B3)</f>
         <v>0 - 20315731330 - 202302 - VARENIZA ANGEL</v>
       </c>
-      <c r="N3" s="3" t="str">
-        <f t="shared" ref="N3:N66" si="4">CONCATENATE(TEXT(A3,"0")," - ",SUBSTITUTE(D3,"-","")," - ",TEXT(K3,"AAAAMM")," - ",B3)</f>
+      <c r="O3" s="3" t="str">
+        <f t="shared" ref="O3:O66" si="4">CONCATENATE(TEXT(A3,"0")," - ",SUBSTITUTE(D3,"-","")," - ",TEXT(L3,"AAAAMM")," - ",B3)</f>
         <v>0 - 20315731330 - 202302 - VARENIZA ANGEL</v>
       </c>
-      <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
-      <c r="R3" s="4">
+      <c r="R3" s="3"/>
+      <c r="S3" s="4">
         <f>ROW(A3)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4">
         <v>20364074310</v>
       </c>
       <c r="D4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E4" s="1">
         <v>44743</v>
       </c>
       <c r="F4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H4" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\BEITIA TOMAS\2022\07\</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="J4" s="4" t="str">
+      <c r="J4" s="4"/>
+      <c r="K4" s="4" t="str">
         <f t="shared" si="2"/>
         <v>202207</v>
       </c>
-      <c r="K4" s="3" t="str">
+      <c r="L4" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E4,"MMMM AAAA"),1))&amp;MID(TEXT(E4,"MMMM AAAA"),2,30)</f>
         <v>Julio 2022</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3" t="str">
+      <c r="M4" s="3"/>
+      <c r="N4" s="3" t="str">
         <f t="shared" si="3"/>
         <v>0 - 20364074310 - 202207 - BEITIA TOMAS</v>
       </c>
-      <c r="N4" s="3" t="str">
+      <c r="O4" s="3" t="str">
         <f t="shared" si="4"/>
         <v>0 - 20364074310 - 202207 - BEITIA TOMAS</v>
       </c>
-      <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
-      <c r="R4" s="4">
+      <c r="R4" s="3"/>
+      <c r="S4" s="4">
         <f>ROW(A4)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5">
         <v>27067089680</v>
       </c>
       <c r="D5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E5" s="1">
         <v>44958</v>
       </c>
       <c r="G5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H5" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\SESMERO TERESITA\2023\02\</v>
       </c>
       <c r="I5" s="4"/>
-      <c r="J5" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K5" s="3" t="str">
+      <c r="J5" s="4"/>
+      <c r="K5" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L5" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E5,"MMMM AAAA"),1))&amp;MID(TEXT(E5,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3" t="str">
+      <c r="M5" s="3"/>
+      <c r="N5" s="3" t="str">
         <f t="shared" si="3"/>
         <v>0 - 27067089680 - 202302 - SESMERO TERESITA</v>
       </c>
-      <c r="N5" s="3" t="str">
+      <c r="O5" s="3" t="str">
         <f t="shared" si="4"/>
         <v>0 - 27067089680 - 202302 - SESMERO TERESITA</v>
       </c>
-      <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
-      <c r="R5" s="4">
+      <c r="R5" s="3"/>
+      <c r="S5" s="4">
         <f>ROW(A5)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6">
         <v>27116976620</v>
       </c>
       <c r="D6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E6" s="1">
         <v>44958</v>
       </c>
       <c r="G6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H6" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\URRUTIA MIRIAM\2023\02\</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K6" s="3" t="str">
+      <c r="J6" s="4"/>
+      <c r="K6" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L6" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E6,"MMMM AAAA"),1))&amp;MID(TEXT(E6,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3" t="str">
+      <c r="M6" s="3"/>
+      <c r="N6" s="3" t="str">
         <f t="shared" si="3"/>
         <v>0 - 27116976620 - 202302 - URRUTIA MIRIAM</v>
       </c>
-      <c r="N6" s="3" t="str">
+      <c r="O6" s="3" t="str">
         <f t="shared" si="4"/>
         <v>0 - 27116976620 - 202302 - URRUTIA MIRIAM</v>
       </c>
-      <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
-      <c r="R6" s="4">
+      <c r="R6" s="3"/>
+      <c r="S6" s="4">
         <f>ROW(A6)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>20133762761</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1">
         <v>44958</v>
       </c>
       <c r="G7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H7" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\MEDINT SRL\2023\02\</v>
       </c>
       <c r="I7" s="4"/>
-      <c r="J7" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K7" s="3" t="str">
+      <c r="J7" s="4"/>
+      <c r="K7" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L7" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E7,"MMMM AAAA"),1))&amp;MID(TEXT(E7,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3" t="str">
+      <c r="M7" s="3"/>
+      <c r="N7" s="3" t="str">
         <f t="shared" si="3"/>
         <v>0 - 30657146850 - 202302 - MEDINT SRL</v>
       </c>
-      <c r="N7" s="3" t="str">
+      <c r="O7" s="3" t="str">
         <f t="shared" si="4"/>
         <v>0 - 30657146850 - 202302 - MEDINT SRL</v>
       </c>
-      <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
-      <c r="R7" s="4">
+      <c r="R7" s="3"/>
+      <c r="S7" s="4">
         <f>ROW(A7)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>20133762761</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="1">
         <v>44958</v>
       </c>
       <c r="G8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H8" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\FERREYRA CARLOS ALFREDO\2023\02\</v>
       </c>
       <c r="I8" s="4"/>
-      <c r="J8" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K8" s="3" t="str">
+      <c r="J8" s="4"/>
+      <c r="K8" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L8" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E8,"MMMM AAAA"),1))&amp;MID(TEXT(E8,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3" t="str">
+      <c r="M8" s="3"/>
+      <c r="N8" s="3" t="str">
         <f t="shared" si="3"/>
         <v>1 - 20133762761 - 202302 - FERREYRA CARLOS ALFREDO</v>
       </c>
-      <c r="N8" s="3" t="str">
+      <c r="O8" s="3" t="str">
         <f t="shared" si="4"/>
         <v>1 - 20133762761 - 202302 - FERREYRA CARLOS ALFREDO</v>
       </c>
-      <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
-      <c r="R8" s="4">
+      <c r="R8" s="3"/>
+      <c r="S8" s="4">
         <f>ROW(A8)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>20149462601</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1">
         <v>44958</v>
       </c>
       <c r="G9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H9" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\SZYCHOWSKI MARCELO\2023\02\</v>
       </c>
       <c r="I9" s="4"/>
-      <c r="J9" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K9" s="3" t="str">
+      <c r="J9" s="4"/>
+      <c r="K9" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L9" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E9,"MMMM AAAA"),1))&amp;MID(TEXT(E9,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3" t="str">
+      <c r="M9" s="3"/>
+      <c r="N9" s="3" t="str">
         <f t="shared" si="3"/>
         <v>1 - 20149462601 - 202302 - SZYCHOWSKI MARCELO</v>
       </c>
-      <c r="N9" s="3" t="str">
+      <c r="O9" s="3" t="str">
         <f t="shared" si="4"/>
         <v>1 - 20149462601 - 202302 - SZYCHOWSKI MARCELO</v>
       </c>
-      <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
-      <c r="R9" s="4">
+      <c r="R9" s="3"/>
+      <c r="S9" s="4">
         <f>ROW(A9)</f>
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>20168291281</v>
@@ -1400,45 +1414,46 @@
         <v>44958</v>
       </c>
       <c r="G10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H10" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\BUSTOS GUSTAVO\2023\02\</v>
       </c>
       <c r="I10" s="4"/>
-      <c r="J10" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K10" s="3" t="str">
+      <c r="J10" s="4"/>
+      <c r="K10" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L10" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E10,"MMMM AAAA"),1))&amp;MID(TEXT(E10,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3" t="str">
+      <c r="M10" s="3"/>
+      <c r="N10" s="3" t="str">
         <f t="shared" si="3"/>
         <v>1 - 20168291281 - 202302 - BUSTOS GUSTAVO</v>
       </c>
-      <c r="N10" s="3" t="str">
+      <c r="O10" s="3" t="str">
         <f t="shared" si="4"/>
         <v>1 - 20168291281 - 202302 - BUSTOS GUSTAVO</v>
       </c>
-      <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
-      <c r="R10" s="4">
+      <c r="R10" s="3"/>
+      <c r="S10" s="4">
         <f>ROW(A10)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <v>20172521771</v>
@@ -1451,345 +1466,352 @@
         <v>44958</v>
       </c>
       <c r="G11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H11" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\PEREYRA ESTEBAN\2023\02\</v>
       </c>
       <c r="I11" s="4"/>
-      <c r="J11" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K11" s="3" t="str">
+      <c r="J11" s="4"/>
+      <c r="K11" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L11" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E11,"MMMM AAAA"),1))&amp;MID(TEXT(E11,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3" t="str">
+      <c r="M11" s="3"/>
+      <c r="N11" s="3" t="str">
         <f t="shared" si="3"/>
         <v>1 - 20172521771 - 202302 - PEREYRA ESTEBAN</v>
       </c>
-      <c r="N11" s="3" t="str">
+      <c r="O11" s="3" t="str">
         <f t="shared" si="4"/>
         <v>1 - 20172521771 - 202302 - PEREYRA ESTEBAN</v>
       </c>
-      <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
-      <c r="R11" s="4">
+      <c r="R11" s="3"/>
+      <c r="S11" s="4">
         <f>ROW(A11)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12">
         <v>27128520851</v>
       </c>
       <c r="D12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E12" s="1">
         <v>44958</v>
       </c>
       <c r="G12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H12" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\MOLAS PATRICIA\2023\02\</v>
       </c>
       <c r="I12" s="4"/>
-      <c r="J12" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K12" s="3" t="str">
+      <c r="J12" s="4"/>
+      <c r="K12" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L12" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E12,"MMMM AAAA"),1))&amp;MID(TEXT(E12,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3" t="str">
+      <c r="M12" s="3"/>
+      <c r="N12" s="3" t="str">
         <f t="shared" si="3"/>
         <v>1 - 27128520851 - 202302 - MOLAS PATRICIA</v>
       </c>
-      <c r="N12" s="3" t="str">
+      <c r="O12" s="3" t="str">
         <f t="shared" si="4"/>
         <v>1 - 27128520851 - 202302 - MOLAS PATRICIA</v>
       </c>
-      <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="4">
+      <c r="R12" s="3"/>
+      <c r="S12" s="4">
         <f>ROW(A12)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13">
         <v>20149466356</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" s="1">
         <v>44958</v>
       </c>
       <c r="G13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H13" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\GESAL SA\2023\02\</v>
       </c>
       <c r="I13" s="4"/>
-      <c r="J13" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K13" s="3" t="str">
+      <c r="J13" s="4"/>
+      <c r="K13" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L13" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E13,"MMMM AAAA"),1))&amp;MID(TEXT(E13,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3" t="str">
+      <c r="M13" s="3"/>
+      <c r="N13" s="3" t="str">
         <f t="shared" si="3"/>
         <v>1 - 30710404131 - 202302 - GESAL SA</v>
       </c>
-      <c r="N13" s="3" t="str">
+      <c r="O13" s="3" t="str">
         <f t="shared" si="4"/>
         <v>1 - 30710404131 - 202302 - GESAL SA</v>
       </c>
-      <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="4">
+      <c r="R13" s="3"/>
+      <c r="S13" s="4">
         <f>ROW(A13)</f>
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14">
         <v>27109797257</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14" s="1">
         <v>44958</v>
       </c>
       <c r="G14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H14" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\CONDOMINIO SAN LORENZO\2023\02\</v>
       </c>
       <c r="I14" s="4"/>
-      <c r="J14" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K14" s="3" t="str">
+      <c r="J14" s="4"/>
+      <c r="K14" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L14" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E14,"MMMM AAAA"),1))&amp;MID(TEXT(E14,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3" t="str">
+      <c r="M14" s="3"/>
+      <c r="N14" s="3" t="str">
         <f t="shared" si="3"/>
         <v>1 - 30717059111 - 202302 - CONDOMINIO SAN LORENZO</v>
       </c>
-      <c r="N14" s="3" t="str">
+      <c r="O14" s="3" t="str">
         <f t="shared" si="4"/>
         <v>1 - 30717059111 - 202302 - CONDOMINIO SAN LORENZO</v>
       </c>
-      <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
-      <c r="R14" s="4">
+      <c r="R14" s="3"/>
+      <c r="S14" s="4">
         <f>ROW(A14)</f>
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C15">
         <v>20121182832</v>
       </c>
       <c r="D15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E15" s="1">
         <v>44958</v>
       </c>
       <c r="G15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H15" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\RIERA HECTOR M\2023\02\</v>
       </c>
       <c r="I15" s="4"/>
-      <c r="J15" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K15" s="3" t="str">
+      <c r="J15" s="4"/>
+      <c r="K15" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L15" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E15,"MMMM AAAA"),1))&amp;MID(TEXT(E15,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3" t="str">
+      <c r="M15" s="3"/>
+      <c r="N15" s="3" t="str">
         <f t="shared" si="3"/>
         <v>2 - 20121182832 - 202302 - RIERA HECTOR M</v>
       </c>
-      <c r="N15" s="3" t="str">
+      <c r="O15" s="3" t="str">
         <f t="shared" si="4"/>
         <v>2 - 20121182832 - 202302 - RIERA HECTOR M</v>
       </c>
-      <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
-      <c r="R15" s="4">
+      <c r="R15" s="3"/>
+      <c r="S15" s="4">
         <f>ROW(A15)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C16">
         <v>20147130202</v>
       </c>
       <c r="D16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E16" s="1">
         <v>44958</v>
       </c>
       <c r="G16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H16" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\BUSTOS MARTIN\2023\02\</v>
       </c>
       <c r="I16" s="4"/>
-      <c r="J16" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K16" s="3" t="str">
+      <c r="J16" s="4"/>
+      <c r="K16" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L16" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E16,"MMMM AAAA"),1))&amp;MID(TEXT(E16,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3" t="str">
+      <c r="M16" s="3"/>
+      <c r="N16" s="3" t="str">
         <f t="shared" si="3"/>
         <v>2 - 20147130202 - 202302 - BUSTOS MARTIN</v>
       </c>
-      <c r="N16" s="3" t="str">
+      <c r="O16" s="3" t="str">
         <f t="shared" si="4"/>
         <v>2 - 20147130202 - 202302 - BUSTOS MARTIN</v>
       </c>
-      <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
-      <c r="R16" s="4">
+      <c r="R16" s="3"/>
+      <c r="S16" s="4">
         <f>ROW(A16)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17">
         <v>20174123072</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E17" s="1">
         <v>44958</v>
       </c>
       <c r="G17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H17" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\INSAURRALDE CARLOS\2023\02\</v>
       </c>
       <c r="I17" s="4"/>
-      <c r="J17" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K17" s="3" t="str">
+      <c r="J17" s="4"/>
+      <c r="K17" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L17" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E17,"MMMM AAAA"),1))&amp;MID(TEXT(E17,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3" t="str">
+      <c r="M17" s="3"/>
+      <c r="N17" s="3" t="str">
         <f t="shared" si="3"/>
         <v>2 - 20174123072 - 202302 - INSAURRALDE CARLOS</v>
       </c>
-      <c r="N17" s="3" t="str">
+      <c r="O17" s="3" t="str">
         <f t="shared" si="4"/>
         <v>2 - 20174123072 - 202302 - INSAURRALDE CARLOS</v>
       </c>
-      <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
-      <c r="R17" s="4">
+      <c r="R17" s="3"/>
+      <c r="S17" s="4">
         <f>ROW(A17)</f>
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18">
         <v>27182653972</v>
@@ -1802,801 +1824,817 @@
         <v>44958</v>
       </c>
       <c r="G18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H18" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\FERNANDEZ SOSA LILIANA\2023\02\</v>
       </c>
       <c r="I18" s="4"/>
-      <c r="J18" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K18" s="3" t="str">
+      <c r="J18" s="4"/>
+      <c r="K18" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L18" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E18,"MMMM AAAA"),1))&amp;MID(TEXT(E18,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3" t="str">
+      <c r="M18" s="3"/>
+      <c r="N18" s="3" t="str">
         <f t="shared" si="3"/>
         <v>2 - 27182653972 - 202302 - FERNANDEZ SOSA LILIANA</v>
       </c>
-      <c r="N18" s="3" t="str">
+      <c r="O18" s="3" t="str">
         <f t="shared" si="4"/>
         <v>2 - 27182653972 - 202302 - FERNANDEZ SOSA LILIANA</v>
       </c>
-      <c r="O18" s="3"/>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
-      <c r="R18" s="4">
+      <c r="R18" s="3"/>
+      <c r="S18" s="4">
         <f>ROW(A18)</f>
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19">
         <v>27348916942</v>
       </c>
       <c r="D19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E19" s="1">
         <v>44743</v>
       </c>
       <c r="F19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H19" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\SZYCHOWSKI KAREN\2022\07\</v>
       </c>
       <c r="I19" s="4"/>
-      <c r="J19" s="4" t="str">
+      <c r="J19" s="4"/>
+      <c r="K19" s="4" t="str">
         <f t="shared" si="2"/>
         <v>202207</v>
       </c>
-      <c r="K19" s="3" t="str">
+      <c r="L19" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E19,"MMMM AAAA"),1))&amp;MID(TEXT(E19,"MMMM AAAA"),2,30)</f>
         <v>Julio 2022</v>
       </c>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3" t="str">
+      <c r="M19" s="3"/>
+      <c r="N19" s="3" t="str">
         <f t="shared" si="3"/>
         <v>2 - 27348916942 - 202207 - SZYCHOWSKI KAREN</v>
       </c>
-      <c r="N19" s="3" t="str">
+      <c r="O19" s="3" t="str">
         <f t="shared" si="4"/>
         <v>2 - 27348916942 - 202207 - SZYCHOWSKI KAREN</v>
       </c>
-      <c r="O19" s="3"/>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
-      <c r="R19" s="4">
+      <c r="R19" s="3"/>
+      <c r="S19" s="4">
         <f>ROW(A19)</f>
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20">
         <v>20100325048</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E20" s="1">
         <v>44958</v>
       </c>
       <c r="G20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H20" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\POSADAS FIDUCIARIA SA\2023\02\</v>
       </c>
       <c r="I20" s="4"/>
-      <c r="J20" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K20" s="3" t="str">
+      <c r="J20" s="4"/>
+      <c r="K20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L20" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E20,"MMMM AAAA"),1))&amp;MID(TEXT(E20,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3" t="str">
+      <c r="M20" s="3"/>
+      <c r="N20" s="3" t="str">
         <f t="shared" si="3"/>
         <v>2 - 30708370122 - 202302 - POSADAS FIDUCIARIA SA</v>
       </c>
-      <c r="N20" s="3" t="str">
+      <c r="O20" s="3" t="str">
         <f t="shared" si="4"/>
         <v>2 - 30708370122 - 202302 - POSADAS FIDUCIARIA SA</v>
       </c>
-      <c r="O20" s="3"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
-      <c r="R20" s="4">
+      <c r="R20" s="3"/>
+      <c r="S20" s="4">
         <f>ROW(A20)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="str">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C21">
         <v>27068286323</v>
       </c>
       <c r="D21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E21" s="1">
         <v>44958</v>
       </c>
       <c r="G21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H21" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\SEMILLA ELVIES\2023\02\</v>
       </c>
       <c r="I21" s="4"/>
-      <c r="J21" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K21" s="3" t="str">
+      <c r="J21" s="4"/>
+      <c r="K21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L21" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E21,"MMMM AAAA"),1))&amp;MID(TEXT(E21,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3" t="str">
+      <c r="M21" s="3"/>
+      <c r="N21" s="3" t="str">
         <f t="shared" si="3"/>
         <v>3 - 27068286323 - 202302 - SEMILLA ELVIES</v>
       </c>
-      <c r="N21" s="3" t="str">
+      <c r="O21" s="3" t="str">
         <f t="shared" si="4"/>
         <v>3 - 27068286323 - 202302 - SEMILLA ELVIES</v>
       </c>
-      <c r="O21" s="3"/>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
-      <c r="R21" s="4">
+      <c r="R21" s="3"/>
+      <c r="S21" s="4">
         <f>ROW(A21)</f>
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="str">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C22">
         <v>27354872183</v>
       </c>
       <c r="D22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E22" s="1">
         <v>44743</v>
       </c>
       <c r="F22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H22" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\PENSA MARIA EUGENIA\2022\07\</v>
       </c>
       <c r="I22" s="4"/>
-      <c r="J22" s="4" t="str">
+      <c r="J22" s="4"/>
+      <c r="K22" s="4" t="str">
         <f t="shared" si="2"/>
         <v>202207</v>
       </c>
-      <c r="K22" s="3" t="str">
+      <c r="L22" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E22,"MMMM AAAA"),1))&amp;MID(TEXT(E22,"MMMM AAAA"),2,30)</f>
         <v>Julio 2022</v>
       </c>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3" t="str">
+      <c r="M22" s="3"/>
+      <c r="N22" s="3" t="str">
         <f t="shared" si="3"/>
         <v>3 - 27354872183 - 202207 - PENSA MARIA EUGENIA</v>
       </c>
-      <c r="N22" s="3" t="str">
+      <c r="O22" s="3" t="str">
         <f t="shared" si="4"/>
         <v>3 - 27354872183 - 202207 - PENSA MARIA EUGENIA</v>
       </c>
-      <c r="O22" s="3"/>
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
-      <c r="R22" s="4">
+      <c r="R22" s="3"/>
+      <c r="S22" s="4">
         <f>ROW(A22)</f>
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="str">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23">
         <v>20114794083</v>
       </c>
       <c r="D23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E23" s="1">
         <v>44958</v>
       </c>
       <c r="G23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H23" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\CUCYTI SRL\2023\02\</v>
       </c>
       <c r="I23" s="4"/>
-      <c r="J23" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K23" s="3" t="str">
+      <c r="J23" s="4"/>
+      <c r="K23" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L23" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E23,"MMMM AAAA"),1))&amp;MID(TEXT(E23,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3" t="str">
+      <c r="M23" s="3"/>
+      <c r="N23" s="3" t="str">
         <f t="shared" si="3"/>
         <v>3 - 30672355393 - 202302 - CUCYTI SRL</v>
       </c>
-      <c r="N23" s="3" t="str">
+      <c r="O23" s="3" t="str">
         <f t="shared" si="4"/>
         <v>3 - 30672355393 - 202302 - CUCYTI SRL</v>
       </c>
-      <c r="O23" s="3"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
-      <c r="R23" s="4">
+      <c r="R23" s="3"/>
+      <c r="S23" s="4">
         <f>ROW(A23)</f>
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="str">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C24">
         <v>23149462074</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E24" s="1">
         <v>44958</v>
       </c>
       <c r="G24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H24" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\CARLOS ABELARDO SESMERO SRL\2023\02\</v>
       </c>
       <c r="I24" s="4"/>
-      <c r="J24" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K24" s="3" t="str">
+      <c r="J24" s="4"/>
+      <c r="K24" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L24" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E24,"MMMM AAAA"),1))&amp;MID(TEXT(E24,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3" t="str">
+      <c r="M24" s="3"/>
+      <c r="N24" s="3" t="str">
         <f t="shared" si="3"/>
         <v>3 - 30707912223 - 202302 - CARLOS ABELARDO SESMERO SRL</v>
       </c>
-      <c r="N24" s="3" t="str">
+      <c r="O24" s="3" t="str">
         <f t="shared" si="4"/>
         <v>3 - 30707912223 - 202302 - CARLOS ABELARDO SESMERO SRL</v>
       </c>
-      <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
-      <c r="R24" s="4">
+      <c r="R24" s="3"/>
+      <c r="S24" s="4">
         <f>ROW(A24)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="str">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25">
         <v>20133762761</v>
       </c>
       <c r="D25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E25" s="1">
         <v>44958</v>
       </c>
       <c r="G25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H25" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\TRANS. MISIONES SA\2023\02\</v>
       </c>
       <c r="I25" s="4"/>
-      <c r="J25" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K25" s="3" t="str">
+      <c r="J25" s="4"/>
+      <c r="K25" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L25" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E25,"MMMM AAAA"),1))&amp;MID(TEXT(E25,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3" t="str">
+      <c r="M25" s="3"/>
+      <c r="N25" s="3" t="str">
         <f t="shared" si="3"/>
         <v>3 - 30715577743 - 202302 - TRANS. MISIONES SA</v>
       </c>
-      <c r="N25" s="3" t="str">
+      <c r="O25" s="3" t="str">
         <f t="shared" si="4"/>
         <v>3 - 30715577743 - 202302 - TRANS. MISIONES SA</v>
       </c>
-      <c r="O25" s="3"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
-      <c r="R25" s="4">
+      <c r="R25" s="3"/>
+      <c r="S25" s="4">
         <f>ROW(A25)</f>
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="str">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C26">
         <v>27201178776</v>
       </c>
       <c r="D26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E26" s="1">
         <v>44958</v>
       </c>
       <c r="G26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H26" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\DON LALO SRL\2023\02\</v>
       </c>
       <c r="I26" s="4"/>
-      <c r="J26" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K26" s="3" t="str">
+      <c r="J26" s="4"/>
+      <c r="K26" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L26" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E26,"MMMM AAAA"),1))&amp;MID(TEXT(E26,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3" t="str">
+      <c r="M26" s="3"/>
+      <c r="N26" s="3" t="str">
         <f t="shared" si="3"/>
         <v>3 - 30717537153 - 202302 - DON LALO SRL</v>
       </c>
-      <c r="N26" s="3" t="str">
+      <c r="O26" s="3" t="str">
         <f t="shared" si="4"/>
         <v>3 - 30717537153 - 202302 - DON LALO SRL</v>
       </c>
-      <c r="O26" s="3"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
-      <c r="R26" s="4">
+      <c r="R26" s="3"/>
+      <c r="S26" s="4">
         <f>ROW(A26)</f>
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="str">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27">
         <v>20168291834</v>
       </c>
       <c r="D27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E27" s="1">
         <v>44958</v>
       </c>
       <c r="G27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H27" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\FERNANDEZ SOSA RODOLFO\2023\02\</v>
       </c>
       <c r="I27" s="4"/>
-      <c r="J27" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K27" s="3" t="str">
+      <c r="J27" s="4"/>
+      <c r="K27" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L27" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E27,"MMMM AAAA"),1))&amp;MID(TEXT(E27,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3" t="str">
+      <c r="M27" s="3"/>
+      <c r="N27" s="3" t="str">
         <f t="shared" si="3"/>
         <v>4 - 20168291834 - 202302 - FERNANDEZ SOSA RODOLFO</v>
       </c>
-      <c r="N27" s="3" t="str">
+      <c r="O27" s="3" t="str">
         <f t="shared" si="4"/>
         <v>4 - 20168291834 - 202302 - FERNANDEZ SOSA RODOLFO</v>
       </c>
-      <c r="O27" s="3"/>
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
-      <c r="R27" s="4">
+      <c r="R27" s="3"/>
+      <c r="S27" s="4">
         <f>ROW(A27)</f>
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="str">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C28">
         <v>23149462074</v>
       </c>
       <c r="D28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E28" s="1">
         <v>44958</v>
       </c>
       <c r="G28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H28" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\SESMERO MARIA GABRIELA\2023\02\</v>
       </c>
       <c r="I28" s="4"/>
-      <c r="J28" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K28" s="3" t="str">
+      <c r="J28" s="4"/>
+      <c r="K28" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L28" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E28,"MMMM AAAA"),1))&amp;MID(TEXT(E28,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3" t="str">
+      <c r="M28" s="3"/>
+      <c r="N28" s="3" t="str">
         <f t="shared" si="3"/>
         <v>4 - 23149462074 - 202302 - SESMERO MARIA GABRIELA</v>
       </c>
-      <c r="N28" s="3" t="str">
+      <c r="O28" s="3" t="str">
         <f t="shared" si="4"/>
         <v>4 - 23149462074 - 202302 - SESMERO MARIA GABRIELA</v>
       </c>
-      <c r="O28" s="3"/>
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
-      <c r="R28" s="4">
+      <c r="R28" s="3"/>
+      <c r="S28" s="4">
         <f>ROW(A28)</f>
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="str">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C29">
         <v>23342751644</v>
       </c>
       <c r="D29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E29" s="1">
         <v>44958</v>
       </c>
       <c r="G29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H29" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\FERREYRA CARMEN VICTORIA\2023\02\</v>
       </c>
       <c r="I29" s="4"/>
-      <c r="J29" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K29" s="3" t="str">
+      <c r="J29" s="4"/>
+      <c r="K29" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L29" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E29,"MMMM AAAA"),1))&amp;MID(TEXT(E29,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3" t="str">
+      <c r="M29" s="3"/>
+      <c r="N29" s="3" t="str">
         <f t="shared" si="3"/>
         <v>4 - 23342751644 - 202302 - FERREYRA CARMEN VICTORIA</v>
       </c>
-      <c r="N29" s="3" t="str">
+      <c r="O29" s="3" t="str">
         <f t="shared" si="4"/>
         <v>4 - 23342751644 - 202302 - FERREYRA CARMEN VICTORIA</v>
       </c>
-      <c r="O29" s="3"/>
       <c r="P29" s="3"/>
       <c r="Q29" s="3"/>
-      <c r="R29" s="4">
+      <c r="R29" s="3"/>
+      <c r="S29" s="4">
         <f>ROW(A29)</f>
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="str">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30">
         <v>23351897074</v>
       </c>
       <c r="D30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E30" s="1">
         <v>44958</v>
       </c>
       <c r="G30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H30" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\SCOTO LUCILA\2023\02\</v>
       </c>
       <c r="I30" s="4"/>
-      <c r="J30" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K30" s="3" t="str">
+      <c r="J30" s="4"/>
+      <c r="K30" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L30" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E30,"MMMM AAAA"),1))&amp;MID(TEXT(E30,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3" t="str">
+      <c r="M30" s="3"/>
+      <c r="N30" s="3" t="str">
         <f t="shared" si="3"/>
         <v>4 - 23351897074 - 202302 - SCOTO LUCILA</v>
       </c>
-      <c r="N30" s="3" t="str">
+      <c r="O30" s="3" t="str">
         <f t="shared" si="4"/>
         <v>4 - 23351897074 - 202302 - SCOTO LUCILA</v>
       </c>
-      <c r="O30" s="3"/>
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
-      <c r="R30" s="4">
+      <c r="R30" s="3"/>
+      <c r="S30" s="4">
         <f>ROW(A30)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="str">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C31">
         <v>27236873744</v>
       </c>
       <c r="D31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E31" s="1">
         <v>44958</v>
       </c>
       <c r="G31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H31" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\TUFRO MALENA\2023\02\</v>
       </c>
       <c r="I31" s="4"/>
-      <c r="J31" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K31" s="3" t="str">
+      <c r="J31" s="4"/>
+      <c r="K31" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L31" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E31,"MMMM AAAA"),1))&amp;MID(TEXT(E31,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3" t="str">
+      <c r="M31" s="3"/>
+      <c r="N31" s="3" t="str">
         <f t="shared" si="3"/>
         <v>4 - 27236873744 - 202302 - TUFRO MALENA</v>
       </c>
-      <c r="N31" s="3" t="str">
+      <c r="O31" s="3" t="str">
         <f t="shared" si="4"/>
         <v>4 - 27236873744 - 202302 - TUFRO MALENA</v>
       </c>
-      <c r="O31" s="3"/>
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
-      <c r="R31" s="4">
+      <c r="R31" s="3"/>
+      <c r="S31" s="4">
         <f>ROW(A31)</f>
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="str">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32">
         <v>20149462601</v>
       </c>
       <c r="D32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E32" s="1">
         <v>44958</v>
       </c>
       <c r="G32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H32" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\DVC SRL\2023\02\</v>
       </c>
       <c r="I32" s="4"/>
-      <c r="J32" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K32" s="3" t="str">
+      <c r="J32" s="4"/>
+      <c r="K32" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L32" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E32,"MMMM AAAA"),1))&amp;MID(TEXT(E32,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3" t="str">
+      <c r="M32" s="3"/>
+      <c r="N32" s="3" t="str">
         <f t="shared" si="3"/>
         <v>4 - 30709431834 - 202302 - DVC SRL</v>
       </c>
-      <c r="N32" s="3" t="str">
+      <c r="O32" s="3" t="str">
         <f t="shared" si="4"/>
         <v>4 - 30709431834 - 202302 - DVC SRL</v>
       </c>
-      <c r="O32" s="3"/>
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
-      <c r="R32" s="4">
+      <c r="R32" s="3"/>
+      <c r="S32" s="4">
         <f>ROW(A32)</f>
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="str">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33">
         <v>20334250327</v>
       </c>
       <c r="D33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E33" s="1">
         <v>44958</v>
       </c>
       <c r="G33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H33" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\VECINAS SRL\2023\02\</v>
       </c>
       <c r="I33" s="4"/>
-      <c r="J33" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K33" s="3" t="str">
+      <c r="J33" s="4"/>
+      <c r="K33" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L33" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E33,"MMMM AAAA"),1))&amp;MID(TEXT(E33,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3" t="str">
+      <c r="M33" s="3"/>
+      <c r="N33" s="3" t="str">
         <f t="shared" si="3"/>
         <v>4 - 30715795864 - 202302 - VECINAS SRL</v>
       </c>
-      <c r="N33" s="3" t="str">
+      <c r="O33" s="3" t="str">
         <f t="shared" si="4"/>
         <v>4 - 30715795864 - 202302 - VECINAS SRL</v>
       </c>
-      <c r="O33" s="3"/>
       <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
-      <c r="R33" s="4">
+      <c r="R33" s="3"/>
+      <c r="S33" s="4">
         <f>ROW(A33)</f>
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34">
         <v>20074827455</v>
@@ -2609,95 +2647,97 @@
         <v>44958</v>
       </c>
       <c r="G34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H34" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\SZYCHOWSKI RICARDO\2023\02\</v>
       </c>
       <c r="I34" s="4"/>
-      <c r="J34" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K34" s="3" t="str">
+      <c r="J34" s="4"/>
+      <c r="K34" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L34" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E34,"MMMM AAAA"),1))&amp;MID(TEXT(E34,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3" t="str">
+      <c r="M34" s="3"/>
+      <c r="N34" s="3" t="str">
         <f t="shared" si="3"/>
         <v>5 - 20074827455 - 202302 - SZYCHOWSKI RICARDO</v>
       </c>
-      <c r="N34" s="3" t="str">
+      <c r="O34" s="3" t="str">
         <f t="shared" si="4"/>
         <v>5 - 20074827455 - 202302 - SZYCHOWSKI RICARDO</v>
       </c>
-      <c r="O34" s="3"/>
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
-      <c r="R34" s="4">
+      <c r="R34" s="3"/>
+      <c r="S34" s="4">
         <f>ROW(A34)</f>
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C35">
         <v>20170394845</v>
       </c>
       <c r="D35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E35" s="1">
         <v>44958</v>
       </c>
       <c r="G35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H35" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\FERREYRA MARCELO\2023\02\</v>
       </c>
       <c r="I35" s="4"/>
-      <c r="J35" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K35" s="3" t="str">
+      <c r="J35" s="4"/>
+      <c r="K35" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L35" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E35,"MMMM AAAA"),1))&amp;MID(TEXT(E35,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3" t="str">
+      <c r="M35" s="3"/>
+      <c r="N35" s="3" t="str">
         <f t="shared" si="3"/>
         <v>5 - 20170394845 - 202302 - FERREYRA MARCELO</v>
       </c>
-      <c r="N35" s="3" t="str">
+      <c r="O35" s="3" t="str">
         <f t="shared" si="4"/>
         <v>5 - 20170394845 - 202302 - FERREYRA MARCELO</v>
       </c>
-      <c r="O35" s="3"/>
       <c r="P35" s="3"/>
       <c r="Q35" s="3"/>
-      <c r="R35" s="4">
+      <c r="R35" s="3"/>
+      <c r="S35" s="4">
         <f>ROW(A35)</f>
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36">
         <v>27148268105</v>
@@ -2710,45 +2750,46 @@
         <v>44958</v>
       </c>
       <c r="G36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H36" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\CANTELI GRACIELA\2023\02\</v>
       </c>
       <c r="I36" s="4"/>
-      <c r="J36" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K36" s="3" t="str">
+      <c r="J36" s="4"/>
+      <c r="K36" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L36" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E36,"MMMM AAAA"),1))&amp;MID(TEXT(E36,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3" t="str">
+      <c r="M36" s="3"/>
+      <c r="N36" s="3" t="str">
         <f t="shared" si="3"/>
         <v>5 - 27148268105 - 202302 - CANTELI GRACIELA</v>
       </c>
-      <c r="N36" s="3" t="str">
+      <c r="O36" s="3" t="str">
         <f t="shared" si="4"/>
         <v>5 - 27148268105 - 202302 - CANTELI GRACIELA</v>
       </c>
-      <c r="O36" s="3"/>
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
-      <c r="R36" s="4">
+      <c r="R36" s="3"/>
+      <c r="S36" s="4">
         <f>ROW(A36)</f>
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C37">
         <v>27171709925</v>
@@ -2761,495 +2802,505 @@
         <v>44958</v>
       </c>
       <c r="G37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H37" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\CORONAS ALINE\2023\02\</v>
       </c>
       <c r="I37" s="4"/>
-      <c r="J37" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K37" s="3" t="str">
+      <c r="J37" s="4"/>
+      <c r="K37" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L37" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E37,"MMMM AAAA"),1))&amp;MID(TEXT(E37,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3" t="str">
+      <c r="M37" s="3"/>
+      <c r="N37" s="3" t="str">
         <f t="shared" si="3"/>
         <v>5 - 27171709925 - 202302 - CORONAS ALINE</v>
       </c>
-      <c r="N37" s="3" t="str">
+      <c r="O37" s="3" t="str">
         <f t="shared" si="4"/>
         <v>5 - 27171709925 - 202302 - CORONAS ALINE</v>
       </c>
-      <c r="O37" s="3"/>
       <c r="P37" s="3"/>
       <c r="Q37" s="3"/>
-      <c r="R37" s="4">
+      <c r="R37" s="3"/>
+      <c r="S37" s="4">
         <f>ROW(A37)</f>
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C38">
         <v>20114794083</v>
       </c>
       <c r="D38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E38" s="1">
         <v>44958</v>
       </c>
       <c r="G38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H38" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\ASOC. SALUD MNES\2023\02\</v>
       </c>
       <c r="I38" s="4"/>
-      <c r="J38" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K38" s="3" t="str">
+      <c r="J38" s="4"/>
+      <c r="K38" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L38" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E38,"MMMM AAAA"),1))&amp;MID(TEXT(E38,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3" t="str">
+      <c r="M38" s="3"/>
+      <c r="N38" s="3" t="str">
         <f t="shared" si="3"/>
         <v>5 - 30708553715 - 202302 - ASOC. SALUD MNES</v>
       </c>
-      <c r="N38" s="3" t="str">
+      <c r="O38" s="3" t="str">
         <f t="shared" si="4"/>
         <v>5 - 30708553715 - 202302 - ASOC. SALUD MNES</v>
       </c>
-      <c r="O38" s="3"/>
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>
-      <c r="R38" s="4">
+      <c r="R38" s="3"/>
+      <c r="S38" s="4">
         <f>ROW(A38)</f>
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="str">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C39">
         <v>20149466356</v>
       </c>
       <c r="D39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E39" s="1">
         <v>44958</v>
       </c>
       <c r="G39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H39" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\ENRIQUEZ RUBEN\2023\02\</v>
       </c>
       <c r="I39" s="4"/>
-      <c r="J39" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K39" s="3" t="str">
+      <c r="J39" s="4"/>
+      <c r="K39" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L39" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E39,"MMMM AAAA"),1))&amp;MID(TEXT(E39,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3" t="str">
+      <c r="M39" s="3"/>
+      <c r="N39" s="3" t="str">
         <f t="shared" si="3"/>
         <v>6 - 20149466356 - 202302 - ENRIQUEZ RUBEN</v>
       </c>
-      <c r="N39" s="3" t="str">
+      <c r="O39" s="3" t="str">
         <f t="shared" si="4"/>
         <v>6 - 20149466356 - 202302 - ENRIQUEZ RUBEN</v>
       </c>
-      <c r="O39" s="3"/>
       <c r="P39" s="3"/>
       <c r="Q39" s="3"/>
-      <c r="R39" s="4">
+      <c r="R39" s="3"/>
+      <c r="S39" s="4">
         <f>ROW(A39)</f>
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="str">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C40">
         <v>20416948926</v>
       </c>
       <c r="D40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E40" s="1">
         <v>44958</v>
       </c>
       <c r="G40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H40" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\BEITIA IÑAKI\2023\02\</v>
       </c>
       <c r="I40" s="4"/>
-      <c r="J40" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K40" s="3" t="str">
+      <c r="J40" s="4"/>
+      <c r="K40" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L40" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E40,"MMMM AAAA"),1))&amp;MID(TEXT(E40,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3" t="str">
+      <c r="M40" s="3"/>
+      <c r="N40" s="3" t="str">
         <f t="shared" si="3"/>
         <v>6 - 20416948926 - 202302 - BEITIA IÑAKI</v>
       </c>
-      <c r="N40" s="3" t="str">
+      <c r="O40" s="3" t="str">
         <f t="shared" si="4"/>
         <v>6 - 20416948926 - 202302 - BEITIA IÑAKI</v>
       </c>
-      <c r="O40" s="3"/>
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
-      <c r="R40" s="4">
+      <c r="R40" s="3"/>
+      <c r="S40" s="4">
         <f>ROW(A40)</f>
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="str">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C41">
         <v>27058846916</v>
       </c>
       <c r="D41" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E41" s="1">
         <v>44958</v>
       </c>
       <c r="G41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H41" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\LAZCOZ VIOLETA\2023\02\</v>
       </c>
       <c r="I41" s="4"/>
-      <c r="J41" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K41" s="3" t="str">
+      <c r="J41" s="4"/>
+      <c r="K41" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L41" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E41,"MMMM AAAA"),1))&amp;MID(TEXT(E41,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3" t="str">
+      <c r="M41" s="3"/>
+      <c r="N41" s="3" t="str">
         <f t="shared" si="3"/>
         <v>6 - 27058846916 - 202302 - LAZCOZ VIOLETA</v>
       </c>
-      <c r="N41" s="3" t="str">
+      <c r="O41" s="3" t="str">
         <f t="shared" si="4"/>
         <v>6 - 27058846916 - 202302 - LAZCOZ VIOLETA</v>
       </c>
-      <c r="O41" s="3"/>
       <c r="P41" s="3"/>
       <c r="Q41" s="3"/>
-      <c r="R41" s="4">
+      <c r="R41" s="3"/>
+      <c r="S41" s="4">
         <f>ROW(A41)</f>
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="str">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C42">
         <v>27201178776</v>
       </c>
       <c r="D42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E42" s="1">
         <v>44958</v>
       </c>
       <c r="G42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H42" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\SZYCHOWSKI AMANDA \2023\02\</v>
       </c>
       <c r="I42" s="4"/>
-      <c r="J42" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K42" s="3" t="str">
+      <c r="J42" s="4"/>
+      <c r="K42" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L42" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E42,"MMMM AAAA"),1))&amp;MID(TEXT(E42,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3" t="str">
+      <c r="M42" s="3"/>
+      <c r="N42" s="3" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">6 - 27201178776 - 202302 - SZYCHOWSKI AMANDA </v>
       </c>
-      <c r="N42" s="3" t="str">
+      <c r="O42" s="3" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">6 - 27201178776 - 202302 - SZYCHOWSKI AMANDA </v>
       </c>
-      <c r="O42" s="3"/>
       <c r="P42" s="3"/>
       <c r="Q42" s="3"/>
-      <c r="R42" s="4">
+      <c r="R42" s="3"/>
+      <c r="S42" s="4">
         <f>ROW(A42)</f>
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="str">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C43">
         <v>27261827366</v>
       </c>
       <c r="D43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E43" s="1">
         <v>44958</v>
       </c>
       <c r="G43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H43" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\CARBALLO GRACIELA\2023\02\</v>
       </c>
       <c r="I43" s="4"/>
-      <c r="J43" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K43" s="3" t="str">
+      <c r="J43" s="4"/>
+      <c r="K43" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L43" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E43,"MMMM AAAA"),1))&amp;MID(TEXT(E43,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3" t="str">
+      <c r="M43" s="3"/>
+      <c r="N43" s="3" t="str">
         <f t="shared" si="3"/>
         <v>6 - 27261827366 - 202302 - CARBALLO GRACIELA</v>
       </c>
-      <c r="N43" s="3" t="str">
+      <c r="O43" s="3" t="str">
         <f t="shared" si="4"/>
         <v>6 - 27261827366 - 202302 - CARBALLO GRACIELA</v>
       </c>
-      <c r="O43" s="3"/>
       <c r="P43" s="3"/>
       <c r="Q43" s="3"/>
-      <c r="R43" s="4">
+      <c r="R43" s="3"/>
+      <c r="S43" s="4">
         <f>ROW(A43)</f>
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="str">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C44">
         <v>20109908852</v>
       </c>
       <c r="D44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E44" s="1">
         <v>44958</v>
       </c>
       <c r="G44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H44" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\PREST. SANAT. SA\2023\02\</v>
       </c>
       <c r="I44" s="4"/>
-      <c r="J44" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K44" s="3" t="str">
+      <c r="J44" s="4"/>
+      <c r="K44" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L44" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E44,"MMMM AAAA"),1))&amp;MID(TEXT(E44,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3" t="str">
+      <c r="M44" s="3"/>
+      <c r="N44" s="3" t="str">
         <f t="shared" si="3"/>
         <v>6 - 30687910636 - 202302 - PREST. SANAT. SA</v>
       </c>
-      <c r="N44" s="3" t="str">
+      <c r="O44" s="3" t="str">
         <f t="shared" si="4"/>
         <v>6 - 30687910636 - 202302 - PREST. SANAT. SA</v>
       </c>
-      <c r="O44" s="3"/>
       <c r="P44" s="3"/>
       <c r="Q44" s="3"/>
-      <c r="R44" s="4">
+      <c r="R44" s="3"/>
+      <c r="S44" s="4">
         <f>ROW(A44)</f>
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="str">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C45">
         <v>23173121539</v>
       </c>
       <c r="D45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E45" s="1">
         <v>44958</v>
       </c>
       <c r="G45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H45" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\CONSULTORIO SAN MARTIN\2023\02\</v>
       </c>
       <c r="I45" s="4"/>
-      <c r="J45" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K45" s="3" t="str">
+      <c r="J45" s="4"/>
+      <c r="K45" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L45" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E45,"MMMM AAAA"),1))&amp;MID(TEXT(E45,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3" t="str">
+      <c r="M45" s="3"/>
+      <c r="N45" s="3" t="str">
         <f t="shared" si="3"/>
         <v>6 - 30715347926 - 202302 - CONSULTORIO SAN MARTIN</v>
       </c>
-      <c r="N45" s="3" t="str">
+      <c r="O45" s="3" t="str">
         <f t="shared" si="4"/>
         <v>6 - 30715347926 - 202302 - CONSULTORIO SAN MARTIN</v>
       </c>
-      <c r="O45" s="3"/>
       <c r="P45" s="3"/>
       <c r="Q45" s="3"/>
-      <c r="R45" s="4">
+      <c r="R45" s="3"/>
+      <c r="S45" s="4">
         <f>ROW(A45)</f>
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="str">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C46">
         <v>20334250327</v>
       </c>
       <c r="D46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E46" s="1">
         <v>44958</v>
       </c>
       <c r="G46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H46" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\PENSA PROPIEDADES\2023\02\</v>
       </c>
       <c r="I46" s="4"/>
-      <c r="J46" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K46" s="3" t="str">
+      <c r="J46" s="4"/>
+      <c r="K46" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L46" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E46,"MMMM AAAA"),1))&amp;MID(TEXT(E46,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3" t="str">
+      <c r="M46" s="3"/>
+      <c r="N46" s="3" t="str">
         <f t="shared" si="3"/>
         <v>6 - 30716503816 - 202302 - PENSA PROPIEDADES</v>
       </c>
-      <c r="N46" s="3" t="str">
+      <c r="O46" s="3" t="str">
         <f t="shared" si="4"/>
         <v>6 - 30716503816 - 202302 - PENSA PROPIEDADES</v>
       </c>
-      <c r="O46" s="3"/>
       <c r="P46" s="3"/>
       <c r="Q46" s="3"/>
-      <c r="R46" s="4">
+      <c r="R46" s="3"/>
+      <c r="S46" s="4">
         <f>ROW(A46)</f>
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C47">
         <v>20077065637</v>
@@ -3262,45 +3313,46 @@
         <v>44958</v>
       </c>
       <c r="G47" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H47" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\PENSA ANIBAL\2023\02\</v>
       </c>
       <c r="I47" s="4"/>
-      <c r="J47" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K47" s="3" t="str">
+      <c r="J47" s="4"/>
+      <c r="K47" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L47" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E47,"MMMM AAAA"),1))&amp;MID(TEXT(E47,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3" t="str">
+      <c r="M47" s="3"/>
+      <c r="N47" s="3" t="str">
         <f t="shared" si="3"/>
         <v>7 - 20077065637 - 202302 - PENSA ANIBAL</v>
       </c>
-      <c r="N47" s="3" t="str">
+      <c r="O47" s="3" t="str">
         <f t="shared" si="4"/>
         <v>7 - 20077065637 - 202302 - PENSA ANIBAL</v>
       </c>
-      <c r="O47" s="3"/>
       <c r="P47" s="3"/>
       <c r="Q47" s="3"/>
-      <c r="R47" s="4">
+      <c r="R47" s="3"/>
+      <c r="S47" s="4">
         <f>ROW(A47)</f>
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C48">
         <v>20130056637</v>
@@ -3313,95 +3365,97 @@
         <v>44958</v>
       </c>
       <c r="G48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H48" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\TABBIA ENRIQUE\2023\02\</v>
       </c>
       <c r="I48" s="4"/>
-      <c r="J48" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K48" s="3" t="str">
+      <c r="J48" s="4"/>
+      <c r="K48" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L48" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E48,"MMMM AAAA"),1))&amp;MID(TEXT(E48,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3" t="str">
+      <c r="M48" s="3"/>
+      <c r="N48" s="3" t="str">
         <f t="shared" si="3"/>
         <v>7 - 20130056637 - 202302 - TABBIA ENRIQUE</v>
       </c>
-      <c r="N48" s="3" t="str">
+      <c r="O48" s="3" t="str">
         <f t="shared" si="4"/>
         <v>7 - 20130056637 - 202302 - TABBIA ENRIQUE</v>
       </c>
-      <c r="O48" s="3"/>
       <c r="P48" s="3"/>
       <c r="Q48" s="3"/>
-      <c r="R48" s="4">
+      <c r="R48" s="3"/>
+      <c r="S48" s="4">
         <f>ROW(A48)</f>
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C49">
         <v>20170395167</v>
       </c>
       <c r="D49" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E49" s="1">
         <v>44958</v>
       </c>
       <c r="G49" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H49" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\HOPE HUGO\2023\02\</v>
       </c>
       <c r="I49" s="4"/>
-      <c r="J49" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K49" s="3" t="str">
+      <c r="J49" s="4"/>
+      <c r="K49" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L49" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E49,"MMMM AAAA"),1))&amp;MID(TEXT(E49,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3" t="str">
+      <c r="M49" s="3"/>
+      <c r="N49" s="3" t="str">
         <f t="shared" si="3"/>
         <v>7 - 20170395167 - 202302 - HOPE HUGO</v>
       </c>
-      <c r="N49" s="3" t="str">
+      <c r="O49" s="3" t="str">
         <f t="shared" si="4"/>
         <v>7 - 20170395167 - 202302 - HOPE HUGO</v>
       </c>
-      <c r="O49" s="3"/>
       <c r="P49" s="3"/>
       <c r="Q49" s="3"/>
-      <c r="R49" s="4">
+      <c r="R49" s="3"/>
+      <c r="S49" s="4">
         <f>ROW(A49)</f>
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C50">
         <v>20301650087</v>
@@ -3414,448 +3468,457 @@
         <v>44958</v>
       </c>
       <c r="G50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H50" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\VARENIZA NESTOR LEONEL\2023\02\</v>
       </c>
       <c r="I50" s="4"/>
-      <c r="J50" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K50" s="3" t="str">
+      <c r="J50" s="4"/>
+      <c r="K50" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L50" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E50,"MMMM AAAA"),1))&amp;MID(TEXT(E50,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3" t="str">
+      <c r="M50" s="3"/>
+      <c r="N50" s="3" t="str">
         <f t="shared" si="3"/>
         <v>7 - 20301650087 - 202302 - VARENIZA NESTOR LEONEL</v>
       </c>
-      <c r="N50" s="3" t="str">
+      <c r="O50" s="3" t="str">
         <f t="shared" si="4"/>
         <v>7 - 20301650087 - 202302 - VARENIZA NESTOR LEONEL</v>
       </c>
-      <c r="O50" s="3"/>
       <c r="P50" s="3"/>
       <c r="Q50" s="3"/>
-      <c r="R50" s="4">
+      <c r="R50" s="3"/>
+      <c r="S50" s="4">
         <f>ROW(A50)</f>
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C51">
         <v>20327623967</v>
       </c>
       <c r="D51" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E51" s="1">
         <v>44958</v>
       </c>
       <c r="G51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H51" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\FERREYRA ANDRES\2023\02\</v>
       </c>
       <c r="I51" s="4"/>
-      <c r="J51" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K51" s="3" t="str">
+      <c r="J51" s="4"/>
+      <c r="K51" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L51" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E51,"MMMM AAAA"),1))&amp;MID(TEXT(E51,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3" t="str">
+      <c r="M51" s="3"/>
+      <c r="N51" s="3" t="str">
         <f t="shared" si="3"/>
         <v>7 - 20327623967 - 202302 - FERREYRA ANDRES</v>
       </c>
-      <c r="N51" s="3" t="str">
+      <c r="O51" s="3" t="str">
         <f t="shared" si="4"/>
         <v>7 - 20327623967 - 202302 - FERREYRA ANDRES</v>
       </c>
-      <c r="O51" s="3"/>
       <c r="P51" s="3"/>
       <c r="Q51" s="3"/>
-      <c r="R51" s="4">
+      <c r="R51" s="3"/>
+      <c r="S51" s="4">
         <f>ROW(A51)</f>
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C52">
         <v>20334250327</v>
       </c>
       <c r="D52" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E52" s="1">
         <v>44743</v>
       </c>
       <c r="F52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H52" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\PENSA LUCIANO\2022\07\</v>
       </c>
       <c r="I52" s="4"/>
-      <c r="J52" s="4" t="str">
+      <c r="J52" s="4"/>
+      <c r="K52" s="4" t="str">
         <f t="shared" si="2"/>
         <v>202207</v>
       </c>
-      <c r="K52" s="3" t="str">
+      <c r="L52" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E52,"MMMM AAAA"),1))&amp;MID(TEXT(E52,"MMMM AAAA"),2,30)</f>
         <v>Julio 2022</v>
       </c>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3" t="str">
+      <c r="M52" s="3"/>
+      <c r="N52" s="3" t="str">
         <f t="shared" si="3"/>
         <v>7 - 20334250327 - 202207 - PENSA LUCIANO</v>
       </c>
-      <c r="N52" s="3" t="str">
+      <c r="O52" s="3" t="str">
         <f t="shared" si="4"/>
         <v>7 - 20334250327 - 202207 - PENSA LUCIANO</v>
       </c>
-      <c r="O52" s="3"/>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
-      <c r="R52" s="4">
+      <c r="R52" s="3"/>
+      <c r="S52" s="4">
         <f>ROW(A52)</f>
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C53">
         <v>27109797257</v>
       </c>
       <c r="D53" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E53" s="1">
         <v>44958</v>
       </c>
       <c r="G53" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H53" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\SCOTTO OLGA MARIA\2023\02\</v>
       </c>
       <c r="I53" s="4"/>
-      <c r="J53" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K53" s="3" t="str">
+      <c r="J53" s="4"/>
+      <c r="K53" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L53" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E53,"MMMM AAAA"),1))&amp;MID(TEXT(E53,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L53" s="3"/>
-      <c r="M53" s="3" t="str">
+      <c r="M53" s="3"/>
+      <c r="N53" s="3" t="str">
         <f t="shared" si="3"/>
         <v>7 - 27109797257 - 202302 - SCOTTO OLGA MARIA</v>
       </c>
-      <c r="N53" s="3" t="str">
+      <c r="O53" s="3" t="str">
         <f t="shared" si="4"/>
         <v>7 - 27109797257 - 202302 - SCOTTO OLGA MARIA</v>
       </c>
-      <c r="O53" s="3"/>
       <c r="P53" s="3"/>
       <c r="Q53" s="3"/>
-      <c r="R53" s="4">
+      <c r="R53" s="3"/>
+      <c r="S53" s="4">
         <f>ROW(A53)</f>
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B54" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C54">
         <v>27217236547</v>
       </c>
       <c r="D54" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E54" s="1">
         <v>44958</v>
       </c>
       <c r="G54" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H54" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\ROKO EUGENIA\2023\02\</v>
       </c>
       <c r="I54" s="4"/>
-      <c r="J54" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K54" s="3" t="str">
+      <c r="J54" s="4"/>
+      <c r="K54" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L54" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E54,"MMMM AAAA"),1))&amp;MID(TEXT(E54,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L54" s="3"/>
-      <c r="M54" s="3" t="str">
+      <c r="M54" s="3"/>
+      <c r="N54" s="3" t="str">
         <f t="shared" si="3"/>
         <v>7 - 27217236547 - 202302 - ROKO EUGENIA</v>
       </c>
-      <c r="N54" s="3" t="str">
+      <c r="O54" s="3" t="str">
         <f t="shared" si="4"/>
         <v>7 - 27217236547 - 202302 - ROKO EUGENIA</v>
       </c>
-      <c r="O54" s="3"/>
       <c r="P54" s="3"/>
       <c r="Q54" s="3"/>
-      <c r="R54" s="4">
+      <c r="R54" s="3"/>
+      <c r="S54" s="4">
         <f>ROW(A54)</f>
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B55" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C55">
         <v>20147130202</v>
       </c>
       <c r="D55" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E55" s="1">
         <v>44958</v>
       </c>
       <c r="G55" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H55" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\BUSTOS-HOPE S.H\2023\02\</v>
       </c>
       <c r="I55" s="4"/>
-      <c r="J55" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K55" s="3" t="str">
+      <c r="J55" s="4"/>
+      <c r="K55" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L55" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E55,"MMMM AAAA"),1))&amp;MID(TEXT(E55,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3" t="str">
+      <c r="M55" s="3"/>
+      <c r="N55" s="3" t="str">
         <f t="shared" si="3"/>
         <v>7 - 30650940667 - 202302 - BUSTOS-HOPE S.H</v>
       </c>
-      <c r="N55" s="3" t="str">
+      <c r="O55" s="3" t="str">
         <f t="shared" si="4"/>
         <v>7 - 30650940667 - 202302 - BUSTOS-HOPE S.H</v>
       </c>
-      <c r="O55" s="3"/>
       <c r="P55" s="3"/>
       <c r="Q55" s="3"/>
-      <c r="R55" s="4">
+      <c r="R55" s="3"/>
+      <c r="S55" s="4">
         <f>ROW(A55)</f>
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C56">
         <v>20174123072</v>
       </c>
       <c r="D56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E56" s="1">
         <v>44958</v>
       </c>
       <c r="G56" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H56" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\CEBAC\2023\02\</v>
       </c>
       <c r="I56" s="4"/>
-      <c r="J56" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K56" s="3" t="str">
+      <c r="J56" s="4"/>
+      <c r="K56" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L56" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E56,"MMMM AAAA"),1))&amp;MID(TEXT(E56,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L56" s="3"/>
-      <c r="M56" s="3" t="str">
+      <c r="M56" s="3"/>
+      <c r="N56" s="3" t="str">
         <f t="shared" si="3"/>
         <v>7 - 30672372697 - 202302 - CEBAC</v>
       </c>
-      <c r="N56" s="3" t="str">
+      <c r="O56" s="3" t="str">
         <f t="shared" si="4"/>
         <v>7 - 30672372697 - 202302 - CEBAC</v>
       </c>
-      <c r="O56" s="3"/>
       <c r="P56" s="3"/>
       <c r="Q56" s="3"/>
-      <c r="R56" s="4">
+      <c r="R56" s="3"/>
+      <c r="S56" s="4">
         <f>ROW(A56)</f>
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C57">
         <v>23183086499</v>
       </c>
       <c r="D57" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E57" s="1">
         <v>44958</v>
       </c>
       <c r="G57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H57" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\AITA S.A.\2023\02\</v>
       </c>
       <c r="I57" s="4"/>
-      <c r="J57" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K57" s="3" t="str">
+      <c r="J57" s="4"/>
+      <c r="K57" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L57" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E57,"MMMM AAAA"),1))&amp;MID(TEXT(E57,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L57" s="3"/>
-      <c r="M57" s="3" t="str">
+      <c r="M57" s="3"/>
+      <c r="N57" s="3" t="str">
         <f t="shared" si="3"/>
         <v>7 - 30709419567 - 202302 - AITA S.A.</v>
       </c>
-      <c r="N57" s="3" t="str">
+      <c r="O57" s="3" t="str">
         <f t="shared" si="4"/>
         <v>7 - 30709419567 - 202302 - AITA S.A.</v>
       </c>
-      <c r="O57" s="3"/>
       <c r="P57" s="3"/>
       <c r="Q57" s="3"/>
-      <c r="R57" s="4">
+      <c r="R57" s="3"/>
+      <c r="S57" s="4">
         <f>ROW(A57)</f>
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B58" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C58">
         <v>27222731416</v>
       </c>
       <c r="D58" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E58" s="1">
         <v>44958</v>
       </c>
       <c r="G58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H58" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\COND. LARZABAL\2023\02\</v>
       </c>
       <c r="I58" s="4"/>
-      <c r="J58" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K58" s="3" t="str">
+      <c r="J58" s="4"/>
+      <c r="K58" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L58" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E58,"MMMM AAAA"),1))&amp;MID(TEXT(E58,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L58" s="3"/>
-      <c r="M58" s="3" t="str">
+      <c r="M58" s="3"/>
+      <c r="N58" s="3" t="str">
         <f t="shared" si="3"/>
         <v>7 - 30712026797 - 202302 - COND. LARZABAL</v>
       </c>
-      <c r="N58" s="3" t="str">
+      <c r="O58" s="3" t="str">
         <f t="shared" si="4"/>
         <v>7 - 30712026797 - 202302 - COND. LARZABAL</v>
       </c>
-      <c r="O58" s="3"/>
       <c r="P58" s="3"/>
       <c r="Q58" s="3"/>
-      <c r="R58" s="4">
+      <c r="R58" s="3"/>
+      <c r="S58" s="4">
         <f>ROW(A58)</f>
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C59">
         <v>20082750488</v>
@@ -3868,45 +3931,46 @@
         <v>44958</v>
       </c>
       <c r="G59" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H59" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\CASTRO OLIVERA CARLOS\2023\02\</v>
       </c>
       <c r="I59" s="4"/>
-      <c r="J59" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K59" s="3" t="str">
+      <c r="J59" s="4"/>
+      <c r="K59" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L59" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E59,"MMMM AAAA"),1))&amp;MID(TEXT(E59,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L59" s="3"/>
-      <c r="M59" s="3" t="str">
+      <c r="M59" s="3"/>
+      <c r="N59" s="3" t="str">
         <f t="shared" si="3"/>
         <v>8 - 20082750488 - 202302 - CASTRO OLIVERA CARLOS</v>
       </c>
-      <c r="N59" s="3" t="str">
+      <c r="O59" s="3" t="str">
         <f t="shared" si="4"/>
         <v>8 - 20082750488 - 202302 - CASTRO OLIVERA CARLOS</v>
       </c>
-      <c r="O59" s="3"/>
       <c r="P59" s="3"/>
       <c r="Q59" s="3"/>
-      <c r="R59" s="4">
+      <c r="R59" s="3"/>
+      <c r="S59" s="4">
         <f>ROW(A59)</f>
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C60">
         <v>20230966738</v>
@@ -3919,445 +3983,454 @@
         <v>44958</v>
       </c>
       <c r="G60" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H60" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\URRUTIA DIEGO\2023\02\</v>
       </c>
       <c r="I60" s="4"/>
-      <c r="J60" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K60" s="3" t="str">
+      <c r="J60" s="4"/>
+      <c r="K60" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L60" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E60,"MMMM AAAA"),1))&amp;MID(TEXT(E60,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L60" s="3"/>
-      <c r="M60" s="3" t="str">
+      <c r="M60" s="3"/>
+      <c r="N60" s="3" t="str">
         <f t="shared" si="3"/>
         <v>8 - 20230966738 - 202302 - URRUTIA DIEGO</v>
       </c>
-      <c r="N60" s="3" t="str">
+      <c r="O60" s="3" t="str">
         <f t="shared" si="4"/>
         <v>8 - 20230966738 - 202302 - URRUTIA DIEGO</v>
       </c>
-      <c r="O60" s="3"/>
       <c r="P60" s="3"/>
       <c r="Q60" s="3"/>
-      <c r="R60" s="4">
+      <c r="R60" s="3"/>
+      <c r="S60" s="4">
         <f>ROW(A60)</f>
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C61">
         <v>20303980378</v>
       </c>
       <c r="D61" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E61" s="1">
         <v>44958</v>
       </c>
       <c r="G61" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H61" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\CASTRO OLIVERA GONZALO\2023\02\</v>
       </c>
       <c r="I61" s="4"/>
-      <c r="J61" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K61" s="3" t="str">
+      <c r="J61" s="4"/>
+      <c r="K61" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L61" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E61,"MMMM AAAA"),1))&amp;MID(TEXT(E61,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L61" s="3"/>
-      <c r="M61" s="3" t="str">
+      <c r="M61" s="3"/>
+      <c r="N61" s="3" t="str">
         <f t="shared" si="3"/>
         <v>8 - 20303980378 - 202302 - CASTRO OLIVERA GONZALO</v>
       </c>
-      <c r="N61" s="3" t="str">
+      <c r="O61" s="3" t="str">
         <f t="shared" si="4"/>
         <v>8 - 20303980378 - 202302 - CASTRO OLIVERA GONZALO</v>
       </c>
-      <c r="O61" s="3"/>
       <c r="P61" s="3"/>
       <c r="Q61" s="3"/>
-      <c r="R61" s="4">
+      <c r="R61" s="3"/>
+      <c r="S61" s="4">
         <f>ROW(A61)</f>
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B62" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C62">
         <v>27163651918</v>
       </c>
       <c r="D62" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E62" s="1">
         <v>44958</v>
       </c>
       <c r="G62" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H62" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\MARTIN ADRIANA\2023\02\</v>
       </c>
       <c r="I62" s="4"/>
-      <c r="J62" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K62" s="3" t="str">
+      <c r="J62" s="4"/>
+      <c r="K62" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L62" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E62,"MMMM AAAA"),1))&amp;MID(TEXT(E62,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L62" s="3"/>
-      <c r="M62" s="3" t="str">
+      <c r="M62" s="3"/>
+      <c r="N62" s="3" t="str">
         <f t="shared" si="3"/>
         <v>8 - 27163651918 - 202302 - MARTIN ADRIANA</v>
       </c>
-      <c r="N62" s="3" t="str">
+      <c r="O62" s="3" t="str">
         <f t="shared" si="4"/>
         <v>8 - 27163651918 - 202302 - MARTIN ADRIANA</v>
       </c>
-      <c r="O62" s="3"/>
       <c r="P62" s="3"/>
       <c r="Q62" s="3"/>
-      <c r="R62" s="4">
+      <c r="R62" s="3"/>
+      <c r="S62" s="4">
         <f>ROW(A62)</f>
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B63" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C63">
         <v>27201932268</v>
       </c>
       <c r="D63" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E63" s="1">
         <v>44958</v>
       </c>
       <c r="G63" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H63" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\SPAGNOLI SUSANA\2023\02\</v>
       </c>
       <c r="I63" s="4"/>
-      <c r="J63" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K63" s="3" t="str">
+      <c r="J63" s="4"/>
+      <c r="K63" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L63" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E63,"MMMM AAAA"),1))&amp;MID(TEXT(E63,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L63" s="3"/>
-      <c r="M63" s="3" t="str">
+      <c r="M63" s="3"/>
+      <c r="N63" s="3" t="str">
         <f t="shared" si="3"/>
         <v>8 - 27201932268 - 202302 - SPAGNOLI SUSANA</v>
       </c>
-      <c r="N63" s="3" t="str">
+      <c r="O63" s="3" t="str">
         <f t="shared" si="4"/>
         <v>8 - 27201932268 - 202302 - SPAGNOLI SUSANA</v>
       </c>
-      <c r="O63" s="3"/>
       <c r="P63" s="3"/>
       <c r="Q63" s="3"/>
-      <c r="R63" s="4">
+      <c r="R63" s="3"/>
+      <c r="S63" s="4">
         <f>ROW(A63)</f>
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C64">
         <v>20175255819</v>
       </c>
       <c r="D64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E64" s="1">
         <v>44958</v>
       </c>
       <c r="G64" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H64" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\FORESTAL SA\2023\02\</v>
       </c>
       <c r="I64" s="4"/>
-      <c r="J64" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K64" s="3" t="str">
+      <c r="J64" s="4"/>
+      <c r="K64" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L64" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E64,"MMMM AAAA"),1))&amp;MID(TEXT(E64,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L64" s="3"/>
-      <c r="M64" s="3" t="str">
+      <c r="M64" s="3"/>
+      <c r="N64" s="3" t="str">
         <f t="shared" si="3"/>
         <v>8 - 30701299538 - 202302 - FORESTAL SA</v>
       </c>
-      <c r="N64" s="3" t="str">
+      <c r="O64" s="3" t="str">
         <f t="shared" si="4"/>
         <v>8 - 30701299538 - 202302 - FORESTAL SA</v>
       </c>
-      <c r="O64" s="3"/>
       <c r="P64" s="3"/>
       <c r="Q64" s="3"/>
-      <c r="R64" s="4">
+      <c r="R64" s="3"/>
+      <c r="S64" s="4">
         <f>ROW(A64)</f>
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B65" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C65">
         <v>20100325048</v>
       </c>
       <c r="D65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E65" s="1">
         <v>44958</v>
       </c>
       <c r="G65" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H65" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\FIDEIC. PDAS INMOB\2023\02\</v>
       </c>
       <c r="I65" s="4"/>
-      <c r="J65" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K65" s="3" t="str">
+      <c r="J65" s="4"/>
+      <c r="K65" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L65" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E65,"MMMM AAAA"),1))&amp;MID(TEXT(E65,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L65" s="3"/>
-      <c r="M65" s="3" t="str">
+      <c r="M65" s="3"/>
+      <c r="N65" s="3" t="str">
         <f t="shared" si="3"/>
         <v>8 - 30708626348 - 202302 - FIDEIC. PDAS INMOB</v>
       </c>
-      <c r="N65" s="3" t="str">
+      <c r="O65" s="3" t="str">
         <f t="shared" si="4"/>
         <v>8 - 30708626348 - 202302 - FIDEIC. PDAS INMOB</v>
       </c>
-      <c r="O65" s="3"/>
       <c r="P65" s="3"/>
       <c r="Q65" s="3"/>
-      <c r="R65" s="4">
+      <c r="R65" s="3"/>
+      <c r="S65" s="4">
         <f>ROW(A65)</f>
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="str">
         <f t="shared" ref="A66:A75" si="5">RIGHT(D66,1)</f>
         <v>9</v>
       </c>
       <c r="B66" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C66">
         <v>20149466739</v>
       </c>
       <c r="D66" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E66" s="1">
         <v>44958</v>
       </c>
       <c r="G66" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H66" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\HOPE RICARDO\2023\02\</v>
       </c>
       <c r="I66" s="4"/>
-      <c r="J66" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>202302</v>
-      </c>
-      <c r="K66" s="3" t="str">
+      <c r="J66" s="4"/>
+      <c r="K66" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>202302</v>
+      </c>
+      <c r="L66" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E66,"MMMM AAAA"),1))&amp;MID(TEXT(E66,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L66" s="3"/>
-      <c r="M66" s="3" t="str">
+      <c r="M66" s="3"/>
+      <c r="N66" s="3" t="str">
         <f t="shared" si="3"/>
         <v>9 - 20149466739 - 202302 - HOPE RICARDO</v>
       </c>
-      <c r="N66" s="3" t="str">
+      <c r="O66" s="3" t="str">
         <f t="shared" si="4"/>
         <v>9 - 20149466739 - 202302 - HOPE RICARDO</v>
       </c>
-      <c r="O66" s="3"/>
       <c r="P66" s="3"/>
       <c r="Q66" s="3"/>
-      <c r="R66" s="4">
+      <c r="R66" s="3"/>
+      <c r="S66" s="4">
         <f>ROW(A66)</f>
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="str">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="B67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C67">
         <v>20175255819</v>
       </c>
       <c r="D67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E67" s="1">
         <v>44958</v>
       </c>
       <c r="G67" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H67" s="4" t="str">
         <f t="shared" ref="H67:H75" si="6">G67&amp;"\"&amp;B67&amp;"\"&amp;YEAR(E67)&amp;"\"&amp;TEXT(MONTH(E67),"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\BEITIA CRISPIN\2023\02\</v>
       </c>
       <c r="I67" s="4"/>
-      <c r="J67" s="4" t="str">
-        <f t="shared" ref="J67:J75" si="7">TEXT(E67,"AAAAMM")</f>
-        <v>202302</v>
-      </c>
-      <c r="K67" s="3" t="str">
+      <c r="J67" s="4"/>
+      <c r="K67" s="4" t="str">
+        <f t="shared" ref="K67:K75" si="7">TEXT(E67,"AAAAMM")</f>
+        <v>202302</v>
+      </c>
+      <c r="L67" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E67,"MMMM AAAA"),1))&amp;MID(TEXT(E67,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L67" s="3"/>
-      <c r="M67" s="3" t="str">
-        <f t="shared" ref="M67:M75" si="8">CONCATENATE(TEXT(A67,"0")," - ",SUBSTITUTE(D67,"-","")," - ",TEXT(K67,"AAAAMM")," - ",B67)</f>
+      <c r="M67" s="3"/>
+      <c r="N67" s="3" t="str">
+        <f t="shared" ref="N67:N75" si="8">CONCATENATE(TEXT(A67,"0")," - ",SUBSTITUTE(D67,"-","")," - ",TEXT(L67,"AAAAMM")," - ",B67)</f>
         <v>9 - 20175255819 - 202302 - BEITIA CRISPIN</v>
       </c>
-      <c r="N67" s="3" t="str">
-        <f t="shared" ref="N67:N75" si="9">CONCATENATE(TEXT(A67,"0")," - ",SUBSTITUTE(D67,"-","")," - ",TEXT(K67,"AAAAMM")," - ",B67)</f>
+      <c r="O67" s="3" t="str">
+        <f t="shared" ref="O67:O75" si="9">CONCATENATE(TEXT(A67,"0")," - ",SUBSTITUTE(D67,"-","")," - ",TEXT(L67,"AAAAMM")," - ",B67)</f>
         <v>9 - 20175255819 - 202302 - BEITIA CRISPIN</v>
       </c>
-      <c r="O67" s="3"/>
       <c r="P67" s="3"/>
       <c r="Q67" s="3"/>
-      <c r="R67" s="4">
+      <c r="R67" s="3"/>
+      <c r="S67" s="4">
         <f>ROW(A67)</f>
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="str">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="B68" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C68">
         <v>20246008109</v>
       </c>
       <c r="D68" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E68" s="1">
         <v>44958</v>
       </c>
       <c r="G68" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H68" s="4" t="str">
         <f t="shared" si="6"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\BUSTOS GONZALO\2023\02\</v>
       </c>
       <c r="I68" s="4"/>
-      <c r="J68" s="4" t="str">
+      <c r="J68" s="4"/>
+      <c r="K68" s="4" t="str">
         <f t="shared" si="7"/>
         <v>202302</v>
       </c>
-      <c r="K68" s="3" t="str">
+      <c r="L68" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E68,"MMMM AAAA"),1))&amp;MID(TEXT(E68,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L68" s="3"/>
-      <c r="M68" s="3" t="str">
+      <c r="M68" s="3"/>
+      <c r="N68" s="3" t="str">
         <f t="shared" si="8"/>
         <v>9 - 20246008109 - 202302 - BUSTOS GONZALO</v>
       </c>
-      <c r="N68" s="3" t="str">
+      <c r="O68" s="3" t="str">
         <f t="shared" si="9"/>
         <v>9 - 20246008109 - 202302 - BUSTOS GONZALO</v>
       </c>
-      <c r="O68" s="3"/>
       <c r="P68" s="3"/>
       <c r="Q68" s="3"/>
-      <c r="R68" s="4">
+      <c r="R68" s="3"/>
+      <c r="S68" s="4">
         <f>ROW(A68)</f>
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="str">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="B69" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C69">
         <v>23120538209</v>
@@ -4370,341 +4443,348 @@
         <v>44958</v>
       </c>
       <c r="G69" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H69" s="4" t="str">
         <f t="shared" si="6"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\LINDSTROM PLINIO\2023\02\</v>
       </c>
       <c r="I69" s="4"/>
-      <c r="J69" s="4" t="str">
+      <c r="J69" s="4"/>
+      <c r="K69" s="4" t="str">
         <f t="shared" si="7"/>
         <v>202302</v>
       </c>
-      <c r="K69" s="3" t="str">
+      <c r="L69" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E69,"MMMM AAAA"),1))&amp;MID(TEXT(E69,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L69" s="3"/>
-      <c r="M69" s="3" t="str">
+      <c r="M69" s="3"/>
+      <c r="N69" s="3" t="str">
         <f t="shared" si="8"/>
         <v>9 - 23120538209 - 202302 - LINDSTROM PLINIO</v>
       </c>
-      <c r="N69" s="3" t="str">
+      <c r="O69" s="3" t="str">
         <f t="shared" si="9"/>
         <v>9 - 23120538209 - 202302 - LINDSTROM PLINIO</v>
       </c>
-      <c r="O69" s="3"/>
       <c r="P69" s="3"/>
       <c r="Q69" s="3"/>
-      <c r="R69" s="4">
+      <c r="R69" s="3"/>
+      <c r="S69" s="4">
         <f>ROW(A69)</f>
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="str">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="B70" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C70">
         <v>23242946669</v>
       </c>
       <c r="D70" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E70" s="1">
         <v>44958</v>
       </c>
       <c r="G70" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H70" s="4" t="str">
         <f t="shared" si="6"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\SOTO GERONIMO\2023\02\</v>
       </c>
       <c r="I70" s="4"/>
-      <c r="J70" s="4" t="str">
+      <c r="J70" s="4"/>
+      <c r="K70" s="4" t="str">
         <f t="shared" si="7"/>
         <v>202302</v>
       </c>
-      <c r="K70" s="3" t="str">
+      <c r="L70" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E70,"MMMM AAAA"),1))&amp;MID(TEXT(E70,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L70" s="3"/>
-      <c r="M70" s="3" t="str">
+      <c r="M70" s="3"/>
+      <c r="N70" s="3" t="str">
         <f t="shared" si="8"/>
         <v>9 - 23242946669 - 202302 - SOTO GERONIMO</v>
       </c>
-      <c r="N70" s="3" t="str">
+      <c r="O70" s="3" t="str">
         <f t="shared" si="9"/>
         <v>9 - 23242946669 - 202302 - SOTO GERONIMO</v>
       </c>
-      <c r="O70" s="3"/>
       <c r="P70" s="3"/>
       <c r="Q70" s="3"/>
-      <c r="R70" s="4">
+      <c r="R70" s="3"/>
+      <c r="S70" s="4">
         <f>ROW(A70)</f>
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="str">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="B71" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C71">
         <v>27173878309</v>
       </c>
       <c r="D71" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E71" s="1">
         <v>44958</v>
       </c>
       <c r="G71" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H71" s="4" t="str">
         <f t="shared" si="6"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\LIONETO CAROLINA\2023\02\</v>
       </c>
       <c r="I71" s="4"/>
-      <c r="J71" s="4" t="str">
+      <c r="J71" s="4"/>
+      <c r="K71" s="4" t="str">
         <f t="shared" si="7"/>
         <v>202302</v>
       </c>
-      <c r="K71" s="3" t="str">
+      <c r="L71" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E71,"MMMM AAAA"),1))&amp;MID(TEXT(E71,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L71" s="3"/>
-      <c r="M71" s="3" t="str">
+      <c r="M71" s="3"/>
+      <c r="N71" s="3" t="str">
         <f t="shared" si="8"/>
         <v>9 - 27173878309 - 202302 - LIONETO CAROLINA</v>
       </c>
-      <c r="N71" s="3" t="str">
+      <c r="O71" s="3" t="str">
         <f t="shared" si="9"/>
         <v>9 - 27173878309 - 202302 - LIONETO CAROLINA</v>
       </c>
-      <c r="O71" s="3"/>
       <c r="P71" s="3"/>
       <c r="Q71" s="3"/>
-      <c r="R71" s="4">
+      <c r="R71" s="3"/>
+      <c r="S71" s="4">
         <f>ROW(A71)</f>
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="str">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="B72" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C72">
         <v>23351897074</v>
       </c>
       <c r="D72" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E72" s="1">
         <v>44958</v>
       </c>
       <c r="G72" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H72" s="4" t="str">
         <f t="shared" si="6"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\COND. INVERNADA\2023\02\</v>
       </c>
       <c r="I72" s="4"/>
-      <c r="J72" s="4" t="str">
+      <c r="J72" s="4"/>
+      <c r="K72" s="4" t="str">
         <f t="shared" si="7"/>
         <v>202302</v>
       </c>
-      <c r="K72" s="3" t="str">
+      <c r="L72" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E72,"MMMM AAAA"),1))&amp;MID(TEXT(E72,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L72" s="3"/>
-      <c r="M72" s="3" t="str">
+      <c r="M72" s="3"/>
+      <c r="N72" s="3" t="str">
         <f t="shared" si="8"/>
         <v>9 - 30715085409 - 202302 - COND. INVERNADA</v>
       </c>
-      <c r="N72" s="3" t="str">
+      <c r="O72" s="3" t="str">
         <f t="shared" si="9"/>
         <v>9 - 30715085409 - 202302 - COND. INVERNADA</v>
       </c>
-      <c r="O72" s="3"/>
       <c r="P72" s="3"/>
       <c r="Q72" s="3"/>
-      <c r="R72" s="4">
+      <c r="R72" s="3"/>
+      <c r="S72" s="4">
         <f>ROW(A72)</f>
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="str">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="B73" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C73">
         <v>20168296011</v>
       </c>
       <c r="D73" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E73" s="1">
         <v>44958</v>
       </c>
       <c r="G73" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H73" s="4" t="str">
         <f t="shared" si="6"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\FAX SRL\2023\02\</v>
       </c>
       <c r="I73" s="4"/>
-      <c r="J73" s="4" t="str">
+      <c r="J73" s="4"/>
+      <c r="K73" s="4" t="str">
         <f t="shared" si="7"/>
         <v>202302</v>
       </c>
-      <c r="K73" s="3" t="str">
+      <c r="L73" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E73,"MMMM AAAA"),1))&amp;MID(TEXT(E73,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L73" s="3"/>
-      <c r="M73" s="3" t="str">
+      <c r="M73" s="3"/>
+      <c r="N73" s="3" t="str">
         <f t="shared" si="8"/>
         <v>9 - 33653520439 - 202302 - FAX SRL</v>
       </c>
-      <c r="N73" s="3" t="str">
+      <c r="O73" s="3" t="str">
         <f t="shared" si="9"/>
         <v>9 - 33653520439 - 202302 - FAX SRL</v>
       </c>
-      <c r="O73" s="3"/>
       <c r="P73" s="3"/>
       <c r="Q73" s="3"/>
-      <c r="R73" s="4">
+      <c r="R73" s="3"/>
+      <c r="S73" s="4">
         <f>ROW(A73)</f>
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="str">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="B74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C74">
         <v>20175255819</v>
       </c>
       <c r="D74" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E74" s="1">
         <v>44958</v>
       </c>
       <c r="G74" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H74" s="4" t="str">
         <f t="shared" si="6"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\KM 0 SA\2023\02\</v>
       </c>
       <c r="I74" s="4"/>
-      <c r="J74" s="4" t="str">
+      <c r="J74" s="4"/>
+      <c r="K74" s="4" t="str">
         <f t="shared" si="7"/>
         <v>202302</v>
       </c>
-      <c r="K74" s="3" t="str">
+      <c r="L74" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E74,"MMMM AAAA"),1))&amp;MID(TEXT(E74,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L74" s="3"/>
-      <c r="M74" s="3" t="str">
+      <c r="M74" s="3"/>
+      <c r="N74" s="3" t="str">
         <f t="shared" si="8"/>
         <v>9 - 33712370829 - 202302 - KM 0 SA</v>
       </c>
-      <c r="N74" s="3" t="str">
+      <c r="O74" s="3" t="str">
         <f t="shared" si="9"/>
         <v>9 - 33712370829 - 202302 - KM 0 SA</v>
       </c>
-      <c r="O74" s="3"/>
       <c r="P74" s="3"/>
       <c r="Q74" s="3"/>
-      <c r="R74" s="4">
+      <c r="R74" s="3"/>
+      <c r="S74" s="4">
         <f>ROW(A74)</f>
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="str">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="B75" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C75">
         <v>20175255819</v>
       </c>
       <c r="D75" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E75" s="1">
         <v>44958</v>
       </c>
       <c r="G75" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H75" s="4" t="str">
         <f t="shared" si="6"/>
         <v>C:\Users\Agustin Bustos\Desktop\Clientes\INMUEBLES SRL\2023\02\</v>
       </c>
       <c r="I75" s="4"/>
-      <c r="J75" s="4" t="str">
+      <c r="J75" s="4"/>
+      <c r="K75" s="4" t="str">
         <f t="shared" si="7"/>
         <v>202302</v>
       </c>
-      <c r="K75" s="3" t="str">
+      <c r="L75" s="3" t="str">
         <f>UPPER(LEFT(TEXT(E75,"MMMM AAAA"),1))&amp;MID(TEXT(E75,"MMMM AAAA"),2,30)</f>
         <v>Febrero 2023</v>
       </c>
-      <c r="L75" s="3"/>
-      <c r="M75" s="3" t="str">
+      <c r="M75" s="3"/>
+      <c r="N75" s="3" t="str">
         <f t="shared" si="8"/>
         <v>9 - 33712529909 - 202302 - INMUEBLES SRL</v>
       </c>
-      <c r="N75" s="3" t="str">
+      <c r="O75" s="3" t="str">
         <f t="shared" si="9"/>
         <v>9 - 33712529909 - 202302 - INMUEBLES SRL</v>
       </c>
-      <c r="O75" s="3"/>
       <c r="P75" s="3"/>
       <c r="Q75" s="3"/>
-      <c r="R75" s="4">
+      <c r="R75" s="3"/>
+      <c r="S75" s="4">
         <f>ROW(A75)</f>
         <v>75</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R75" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S75">
+  <autoFilter ref="A1:S75" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T75">
     <sortCondition ref="B2:B75"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix URL. VER CT
</commit_message>
<xml_diff>
--- a/Importación RETPER SOS.xlsx
+++ b/Importación RETPER SOS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC62CA3-C219-4CD7-A733-CBE361213FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11AC1CD7-B8DB-4575-A988-C59A10521821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -960,7 +960,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U2" sqref="U2"/>
+      <selection pane="bottomLeft" activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>